<commit_message>
Update for for rq tryout 1.0
</commit_message>
<xml_diff>
--- a/wsb_data.xlsx
+++ b/wsb_data.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,6 +441,11 @@
           <t>Comment</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Parent_ID</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -453,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +482,11 @@
           <t>Comment</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Parent_ID</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -489,7 +499,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,6 +523,11 @@
           <t>Comment</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Parent_ID</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -525,7 +540,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,6 +564,11 @@
           <t>Comment</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Parent_ID</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -561,7 +581,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -585,6 +605,11 @@
           <t>Comment</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Parent_ID</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>